<commit_message>
Updated the test spec document.
</commit_message>
<xml_diff>
--- a/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
+++ b/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="696" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="696" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="10.証明書ストア" sheetId="11" r:id="rId13"/>
     <sheet name="11.証明書失効ディレクトリ" sheetId="12" r:id="rId14"/>
     <sheet name="12.tls_cipher_suite" sheetId="15" r:id="rId15"/>
+    <sheet name="13.proxy cert" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="371">
   <si>
     <t>証明書</t>
     <rPh sb="0" eb="3">
@@ -2073,22 +2074,12 @@
   </si>
   <si>
     <t>テストクライアント起動
-% ./tls-test --allow_no_crl --mutual_authentication --tls_certificate_file ./test_dir/permission_crl_dir/B/client/client.crt --tls_key_file ./test_dir/permission_crl_dir/B/client/client.key  --tls_ca_certificate_path ./test_dir/permission_crl_dir/B/cacerts_all --tls_ca_revocation_path ./test_dir/permission_crl_dir/A/crls/server/root/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストクライアント起動
 % ./tls-test --allow_no_crl --mutual_authentication --tls_certificate_file ./test_dir/permission_crl_dir/B/client/client.crt --tls_key_file ./test_dir/permission_crl_dir/B/client/client.key  --tls_ca_certificate_path ./test_dir/permission_crl_dir/B/cacerts_all --tls_ca_revocation_path ./test_dir/permission_crl_dir/A/crls/server/root_bad_permissions</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>テストクライアント起動
 % ./tls-test --allow_no_crl --tls_certificate_file ./test_dir/A/client/client.crt --tls_key_file ./test_dir/A/client/client.key --tls_ca_certificate_path ./test_dir/A/cacerts_all --tls_cipher_suite TLS_AES_128_GCM_SHA256:TLS_CHACHA20_POLY1305_SHA256:TLS_AES_128_CCM_SHA256:TLS_AES_128_CCM_8_SHA256</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストクライアント起動
-% ./tls-test --allow_no_crl --tls_certificate_file ./test_dir/A/client/client.crt --tls_key_file ./test_dir/A/client/client.key --tls_ca_certificate_path ./test_dir/A/cacerts_all --tls_cipher_suite TLS_AES_256_GCM_SHA384</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2348,6 +2339,242 @@
     <t>certs-chain_test.xlsx を参照</t>
     <rPh sb="23" eb="25">
       <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tls_cipher_suite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オプション</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proxy cert</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>* クライアント proxy 証明書: A</t>
+    <rPh sb="15" eb="18">
+      <t>ショウメイショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --allow_no_crl --mutual_authentication --tls_certificate_file ./test_dir/permission_crl_dir/B/client/client.crt --tls_key_file ./test_dir/permission_crl_dir/B/client/client.key  --tls_ca_certificate_path ./test_dir/permission_crl_dir/B/cacerts_all --tls_ca_revocation_path ./test_dir/permission_crl_dir/A/crls/server/root/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13-10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --proxy_cert --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --proxy_cert --mutual_authentication
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --allow_no_crl --tls_certificate_file ./test_dir/A/client/client.crt --tls_key_file ./test_dir/A/client/client.key --tls_ca_certificate_path ./test_dir/A/cacerts_all --tls_cipher_suite TLS_AES_256_GCM_SHA384</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% X509_USER_PROXY=./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --proxy_cert --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">テストクライアント起動
+% cp ./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt /tmp/x509up_u${UID}
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --proxy_cert --mutual_authentication
+% rm /tmp/x509up_u${UID}
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% cp ./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt /tmp/x509up_u${UID}
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --proxy_cert --mutual_authentication
+% rm /tmp/x509up_u${UID}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">テストクライアント起動
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/client_under_root/client.crt --tls_key_file test_dir/proxy_cert/A/client_under_root/client.key --mutual_authentication
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">テストクライアント起動
+% X509_USER_PROXY=./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/client_under_root/client.crt --tls_key_file test_dir/proxy_cert/A/client_under_root/client.key --mutual_authentication
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% X509_USER_PROXY=./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/client_under_root/client.crt --tls_key_file test_dir/proxy_cert/A/client_under_root/client.key --proxy_cert --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/server_under_root/server.crt --tls_key_file test_dir/proxy_cert/A/server_under_root/server.key --build_chain --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% cp ./test_dir/proxy_cert/A/client_under_root/client_cat_all_bad_permissions.crt /tmp/x509up_u${UID}
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --proxy_cert --mutual_authentication
+% rm /tmp/x509up_u${UID}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">テストクライアント起動
+% X509_USER_PROXY=./test_dir/proxy_cert/A/client_under_root/client_cat_all.crt ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/client_under_root/client.crt --tls_key_file test_dir/proxy_cert/A/client_under_root/client.key --proxy_cert --mutual_authentication
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --once --verify_only --allow_no_crl --debug_level 1 --tls_ca_certificate_path test_dir/proxy_cert/A/cacerts_root/ --tls_certificate_file test_dir/proxy_cert/A/client_under_root/client.crt --tls_key_file test_dir/proxy_cert/A/client_under_root/client.key --proxy_cert --mutual_authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>client 側 proxy 指定なし</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">client 側 proxy 指定あり (環境変数) </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">client 側 proxy 指定あり (ファイル) </t>
+  </si>
+  <si>
+    <t>server 側 proxy 指定なし</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>client は proxy 指定ありだが
+server は proxy 指定なし</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proxy cert ファイルが正しく設定され、server, client 双方で proxy 指定</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">proxy cert ファイルのパーミッション 644 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proxy cert ファイルなし、client に proxy 設定あり/user cert あり、server 側 にproxy 指定なしで user cert 認証成功するか</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proxy cert ファイルなし、client に proxy 設定なし/user cert あり、server 側 にproxy 指定なしで user cert 認証成功するか</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proxy cert ファイルあり、client に proxy 設定なし/user cert あり、server 側 にproxy 指定なしで user cert 認証成功するか</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーで起動しないこと</t>
+    <rPh sb="4" eb="6">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>認証に成功すること</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>認証に失敗すること</t>
+    <rPh sb="3" eb="5">
+      <t>シッパイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバの log に "a TLS session established with proxy certificate"  が存在すること</t>
+    <rPh sb="67" eb="69">
+      <t>ソンザイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストサーバの log に "a TLS session established with end-entity certificate"  が存在すること</t>
+    <rPh sb="72" eb="74">
+      <t>ソンザイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2594,7 +2821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2809,6 +3036,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4111,9 +4375,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4123,7 +4387,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -4135,7 +4399,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -4145,7 +4409,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>109</v>
@@ -4157,7 +4421,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -4167,7 +4431,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -4179,7 +4443,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -4189,7 +4453,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
@@ -4201,7 +4465,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
@@ -4213,7 +4477,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4223,7 +4487,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -4235,7 +4499,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3" t="s">
@@ -4247,7 +4511,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
@@ -4257,7 +4521,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
@@ -4269,7 +4533,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
@@ -4281,7 +4545,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
@@ -4291,7 +4555,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>43</v>
@@ -4303,7 +4567,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="3" t="s">
@@ -4315,7 +4579,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="3"/>
@@ -4325,7 +4589,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
@@ -4335,17 +4599,17 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="5"/>
@@ -4356,7 +4620,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4367,7 +4631,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
@@ -4378,7 +4642,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="5"/>
@@ -4389,7 +4653,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="5"/>
@@ -4400,7 +4664,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="5"/>
@@ -4411,7 +4675,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4422,7 +4686,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4433,7 +4697,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
@@ -4444,7 +4708,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4455,7 +4719,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4466,7 +4730,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4477,7 +4741,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4502,17 +4766,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.375" customWidth="1"/>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="82.5" customWidth="1"/>
+    <col min="5" max="5" width="30.75" customWidth="1"/>
+    <col min="7" max="7" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4521,7 +4785,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -4530,7 +4794,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>37</v>
@@ -4539,7 +4803,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>38</v>
@@ -4548,14 +4812,14 @@
       <c r="D4" s="6"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
@@ -4576,7 +4840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>77</v>
       </c>
@@ -4587,7 +4851,7 @@
         <v>225</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>224</v>
@@ -4597,7 +4861,7 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A8" s="30"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -4619,19 +4883,19 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="42.08984375" customWidth="1"/>
-    <col min="3" max="3" width="39.90625" customWidth="1"/>
+    <col min="2" max="2" width="42.125" customWidth="1"/>
+    <col min="3" max="3" width="39.875" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4642,7 +4906,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -4653,7 +4917,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>37</v>
@@ -4663,7 +4927,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>38</v>
@@ -4674,7 +4938,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>89</v>
       </c>
@@ -4685,7 +4949,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>177</v>
@@ -4696,7 +4960,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>137</v>
@@ -4707,7 +4971,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>178</v>
@@ -4718,7 +4982,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
         <v>217</v>
@@ -4729,7 +4993,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>168</v>
       </c>
@@ -4740,7 +5004,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>268</v>
@@ -4751,7 +5015,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -4760,7 +5024,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
@@ -4781,7 +5045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A14" s="68" t="s">
         <v>151</v>
       </c>
@@ -4798,11 +5062,11 @@
         <v>93</v>
       </c>
       <c r="F14" s="71" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G14" s="75"/>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A15" s="44" t="s">
         <v>78</v>
       </c>
@@ -4819,11 +5083,11 @@
         <v>94</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A16" s="56" t="s">
         <v>79</v>
       </c>
@@ -4840,11 +5104,11 @@
         <v>94</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A17" s="56" t="s">
         <v>218</v>
       </c>
@@ -4861,7 +5125,7 @@
         <v>94</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G17" s="21"/>
     </row>
@@ -4879,18 +5143,18 @@
       <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
-    <col min="2" max="2" width="39.6328125" customWidth="1"/>
-    <col min="3" max="3" width="34.6328125" customWidth="1"/>
-    <col min="4" max="4" width="64.08984375" customWidth="1"/>
-    <col min="5" max="5" width="27.26953125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="39.625" customWidth="1"/>
+    <col min="3" max="3" width="34.625" customWidth="1"/>
+    <col min="4" max="4" width="64.125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -4901,7 +5165,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>37</v>
@@ -4912,7 +5176,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>38</v>
@@ -4923,7 +5187,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>92</v>
       </c>
@@ -4934,7 +5198,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
         <v>181</v>
@@ -4945,7 +5209,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>95</v>
@@ -4956,7 +5220,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>171</v>
       </c>
@@ -4967,10 +5231,10 @@
       <c r="F7" s="10"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -4978,7 +5242,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -4987,7 +5251,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -5008,7 +5272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A11" s="76" t="s">
         <v>80</v>
       </c>
@@ -5019,7 +5283,7 @@
         <v>97</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E11" s="69" t="s">
         <v>93</v>
@@ -5029,7 +5293,7 @@
       </c>
       <c r="G11" s="70"/>
     </row>
-    <row r="12" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A12" s="77" t="s">
         <v>172</v>
       </c>
@@ -5050,7 +5314,7 @@
       </c>
       <c r="G12" s="70"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -5059,7 +5323,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -5068,7 +5332,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -5077,7 +5341,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -5086,7 +5350,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -5110,18 +5374,18 @@
       <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
-    <col min="2" max="2" width="44.36328125" customWidth="1"/>
-    <col min="3" max="3" width="37.36328125" customWidth="1"/>
-    <col min="4" max="4" width="71.6328125" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="44.375" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="4" max="4" width="71.625" customWidth="1"/>
+    <col min="5" max="5" width="25.625" customWidth="1"/>
+    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -5132,7 +5396,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10"/>
       <c r="B2" s="19" t="s">
         <v>37</v>
@@ -5143,7 +5407,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="19" t="s">
         <v>39</v>
@@ -5154,7 +5418,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>91</v>
       </c>
@@ -5166,7 +5430,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
         <v>182</v>
@@ -5178,7 +5442,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
@@ -5190,7 +5454,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" s="55" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="55" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>140</v>
@@ -5201,9 +5465,9 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="19"/>
@@ -5212,10 +5476,10 @@
       <c r="F8" s="10"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -5223,7 +5487,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -5232,7 +5496,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
@@ -5253,7 +5517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A12" s="68" t="s">
         <v>152</v>
       </c>
@@ -5264,7 +5528,7 @@
         <v>103</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E12" s="71" t="s">
         <v>93</v>
@@ -5274,7 +5538,7 @@
       </c>
       <c r="G12" s="70"/>
     </row>
-    <row r="13" spans="1:8" ht="65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A13" s="68" t="s">
         <v>173</v>
       </c>
@@ -5295,7 +5559,7 @@
       </c>
       <c r="G13" s="70"/>
     </row>
-    <row r="14" spans="1:8" ht="78" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A14" s="56" t="s">
         <v>174</v>
       </c>
@@ -5306,7 +5570,7 @@
         <v>139</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E14" s="57" t="s">
         <v>93</v>
@@ -5326,22 +5590,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="44.7265625" customWidth="1"/>
-    <col min="4" max="4" width="67.7265625" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="33.375" customWidth="1"/>
+    <col min="3" max="3" width="44.75" customWidth="1"/>
+    <col min="4" max="4" width="67.75" customWidth="1"/>
+    <col min="5" max="5" width="32.875" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="22.90625" customWidth="1"/>
+    <col min="7" max="7" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -5352,7 +5616,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10"/>
       <c r="B2" s="19" t="s">
         <v>37</v>
@@ -5363,7 +5627,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="19" t="s">
         <v>39</v>
@@ -5374,7 +5638,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>141</v>
       </c>
@@ -5385,7 +5649,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="s">
         <v>222</v>
@@ -5396,7 +5660,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>169</v>
@@ -5407,7 +5671,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>142</v>
@@ -5418,7 +5682,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>170</v>
@@ -5429,7 +5693,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>216</v>
       </c>
@@ -5440,10 +5704,10 @@
       <c r="F9" s="10"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -5451,7 +5715,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="19"/>
@@ -5460,7 +5724,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
@@ -5481,7 +5745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>153</v>
       </c>
@@ -5492,7 +5756,7 @@
         <v>144</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>221</v>
@@ -5502,7 +5766,7 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>154</v>
       </c>
@@ -5513,7 +5777,7 @@
         <v>146</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>175</v>
@@ -5523,7 +5787,7 @@
       </c>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>155</v>
       </c>
@@ -5534,7 +5798,7 @@
         <v>148</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>274</v>
+        <v>327</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>93</v>
@@ -5544,7 +5808,7 @@
       </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>156</v>
       </c>
@@ -5555,7 +5819,7 @@
         <v>150</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>176</v>
@@ -5565,10 +5829,10 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="29.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="33.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="29.45" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="28.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="33.6" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5581,20 +5845,20 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.26953125" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="69.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5603,7 +5867,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -5612,7 +5876,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>37</v>
@@ -5621,7 +5885,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>38</v>
@@ -5630,14 +5894,14 @@
       <c r="D4" s="6"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
@@ -5658,7 +5922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>234</v>
       </c>
@@ -5667,28 +5931,28 @@
         <v>240</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>241</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A8" s="30"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" ht="78" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>239</v>
       </c>
@@ -5697,26 +5961,399 @@
         <v>236</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>235</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="30"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="21" t="s">
-        <v>277</v>
+        <v>343</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="21"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="D12:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.25" style="80" customWidth="1"/>
+    <col min="2" max="2" width="27.875" style="80" customWidth="1"/>
+    <col min="3" max="3" width="31.75" style="80" customWidth="1"/>
+    <col min="4" max="4" width="70.375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="27.625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="32.75" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="83"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B2" s="80" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B3" s="80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B4" s="80" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="82"/>
+      <c r="D6" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="84" t="s">
+        <v>328</v>
+      </c>
+      <c r="B7" s="84"/>
+      <c r="C7" s="88" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A8" s="90" t="s">
+        <v>329</v>
+      </c>
+      <c r="B8" s="90"/>
+      <c r="C8" s="86" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="85" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A10" s="90" t="s">
+        <v>330</v>
+      </c>
+      <c r="B10" s="90"/>
+      <c r="C10" s="86" t="s">
+        <v>357</v>
+      </c>
+      <c r="D10" s="85" t="s">
+        <v>338</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A12" s="90" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="90"/>
+      <c r="C12" s="86" t="s">
+        <v>358</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A13" s="91"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A14" s="90" t="s">
+        <v>332</v>
+      </c>
+      <c r="B14" s="90"/>
+      <c r="C14" s="86" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" s="85" t="s">
+        <v>340</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="85" t="s">
+        <v>353</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A16" s="90" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="90"/>
+      <c r="C16" s="86" t="s">
+        <v>360</v>
+      </c>
+      <c r="D16" s="85" t="s">
+        <v>341</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="85" t="s">
+        <v>350</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="84"/>
+      <c r="C18" s="88" t="s">
+        <v>361</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A19" s="90" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="90"/>
+      <c r="C19" s="86" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="85" t="s">
+        <v>354</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A21" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="B21" s="90"/>
+      <c r="C21" s="86" t="s">
+        <v>363</v>
+      </c>
+      <c r="D21" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="85" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A23" s="90" t="s">
+        <v>337</v>
+      </c>
+      <c r="B23" s="90"/>
+      <c r="C23" s="86" t="s">
+        <v>364</v>
+      </c>
+      <c r="D23" s="85" t="s">
+        <v>342</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="85" t="s">
+        <v>349</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -5733,62 +6370,62 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>81</v>
       </c>
@@ -5808,7 +6445,7 @@
       <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5817,20 +6454,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" customWidth="1"/>
-    <col min="3" max="3" width="37.36328125" customWidth="1"/>
-    <col min="4" max="4" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -5844,7 +6481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5855,10 +6492,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5868,7 +6505,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5878,7 +6515,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5888,7 +6525,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5898,7 +6535,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5908,7 +6545,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5918,7 +6555,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5930,7 +6567,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5940,7 +6577,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5950,7 +6587,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5959,6 +6596,30 @@
         <v>157</v>
       </c>
       <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="79">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="79" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -5971,23 +6632,23 @@
   <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" style="19" customWidth="1"/>
-    <col min="2" max="3" width="26.6328125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.08984375" style="19" customWidth="1"/>
-    <col min="5" max="6" width="28.90625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="76.7265625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="20.90625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="29.453125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="19"/>
+    <col min="1" max="1" width="8.125" style="19" customWidth="1"/>
+    <col min="2" max="3" width="26.625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="19" customWidth="1"/>
+    <col min="5" max="6" width="28.875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="76.75" style="19" customWidth="1"/>
+    <col min="8" max="8" width="20.875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="19" customWidth="1"/>
+    <col min="10" max="10" width="29.5" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.75" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5996,7 +6657,7 @@
       <c r="D1" s="10"/>
       <c r="G1" s="35"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -6004,7 +6665,7 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>37</v>
@@ -6012,7 +6673,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>39</v>
@@ -6020,7 +6681,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>83</v>
       </c>
@@ -6028,7 +6689,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>84</v>
@@ -6036,7 +6697,7 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>186</v>
@@ -6044,7 +6705,7 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="28" t="s">
         <v>190</v>
@@ -6052,7 +6713,7 @@
       <c r="C8" s="28"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="28" t="s">
         <v>205</v>
@@ -6060,7 +6721,7 @@
       <c r="C9" s="28"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="28" t="s">
         <v>206</v>
@@ -6068,7 +6729,7 @@
       <c r="C10" s="28"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="24"/>
       <c r="B11" s="28" t="s">
         <v>191</v>
@@ -6082,7 +6743,7 @@
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
     </row>
-    <row r="12" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="24"/>
       <c r="B12" s="28" t="s">
         <v>192</v>
@@ -6096,7 +6757,7 @@
       <c r="J12" s="26"/>
       <c r="K12" s="26"/>
     </row>
-    <row r="13" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="24"/>
       <c r="B13" s="28" t="s">
         <v>202</v>
@@ -6110,7 +6771,7 @@
       <c r="J13" s="26"/>
       <c r="K13" s="26"/>
     </row>
-    <row r="14" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="24"/>
       <c r="B14" s="28" t="s">
         <v>203</v>
@@ -6124,7 +6785,7 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
     </row>
-    <row r="15" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="24"/>
       <c r="B15" s="28" t="s">
         <v>204</v>
@@ -6138,13 +6799,13 @@
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
         <v>12</v>
       </c>
@@ -6168,7 +6829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A18" s="29" t="s">
         <v>14</v>
       </c>
@@ -6188,7 +6849,7 @@
         <v>196</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>187</v>
@@ -6198,7 +6859,7 @@
       </c>
       <c r="J18" s="21"/>
     </row>
-    <row r="19" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A19" s="66"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -6212,7 +6873,7 @@
       <c r="I19" s="27"/>
       <c r="J19" s="21"/>
     </row>
-    <row r="20" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A20" s="66"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -6222,7 +6883,7 @@
         <v>197</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>187</v>
@@ -6232,7 +6893,7 @@
       </c>
       <c r="J20" s="21"/>
     </row>
-    <row r="21" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A21" s="66"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -6246,7 +6907,7 @@
       <c r="I21" s="27"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A22" s="66"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -6256,7 +6917,7 @@
         <v>198</v>
       </c>
       <c r="G22" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H22" s="22" t="s">
         <v>187</v>
@@ -6266,7 +6927,7 @@
       </c>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A23" s="30"/>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -6280,7 +6941,7 @@
       <c r="I23" s="27"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A24" s="29" t="s">
         <v>15</v>
       </c>
@@ -6294,7 +6955,7 @@
         <v>196</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H24" s="22" t="s">
         <v>18</v>
@@ -6304,7 +6965,7 @@
       </c>
       <c r="J24" s="27"/>
     </row>
-    <row r="25" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A25" s="66"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -6318,7 +6979,7 @@
       <c r="I25" s="27"/>
       <c r="J25" s="21"/>
     </row>
-    <row r="26" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A26" s="66"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -6328,7 +6989,7 @@
         <v>197</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H26" s="22" t="s">
         <v>50</v>
@@ -6338,7 +6999,7 @@
       </c>
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A27" s="66"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -6352,7 +7013,7 @@
       <c r="I27" s="27"/>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A28" s="66"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -6362,7 +7023,7 @@
         <v>198</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H28" s="22" t="s">
         <v>50</v>
@@ -6372,7 +7033,7 @@
       </c>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A29" s="66"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -6386,7 +7047,7 @@
       <c r="I29" s="27"/>
       <c r="J29" s="21"/>
     </row>
-    <row r="30" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A30" s="29" t="s">
         <v>207</v>
       </c>
@@ -6400,7 +7061,7 @@
         <v>196</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H30" s="22" t="s">
         <v>50</v>
@@ -6410,7 +7071,7 @@
       </c>
       <c r="J30" s="27"/>
     </row>
-    <row r="31" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A31" s="66"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -6424,7 +7085,7 @@
       <c r="I31" s="27"/>
       <c r="J31" s="21"/>
     </row>
-    <row r="32" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A32" s="66"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
@@ -6434,7 +7095,7 @@
         <v>197</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H32" s="22" t="s">
         <v>18</v>
@@ -6444,7 +7105,7 @@
       </c>
       <c r="J32" s="21"/>
     </row>
-    <row r="33" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A33" s="66"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
@@ -6458,7 +7119,7 @@
       <c r="I33" s="27"/>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A34" s="66"/>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -6468,7 +7129,7 @@
         <v>198</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H34" s="22" t="s">
         <v>50</v>
@@ -6478,7 +7139,7 @@
       </c>
       <c r="J34" s="21"/>
     </row>
-    <row r="35" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A35" s="66"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -6492,7 +7153,7 @@
       <c r="I35" s="27"/>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A36" s="29" t="s">
         <v>210</v>
       </c>
@@ -6506,7 +7167,7 @@
         <v>196</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H36" s="22" t="s">
         <v>50</v>
@@ -6516,7 +7177,7 @@
       </c>
       <c r="J36" s="27"/>
     </row>
-    <row r="37" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A37" s="66"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -6530,7 +7191,7 @@
       <c r="I37" s="27"/>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A38" s="66"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
@@ -6540,7 +7201,7 @@
         <v>197</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H38" s="22" t="s">
         <v>50</v>
@@ -6550,7 +7211,7 @@
       </c>
       <c r="J38" s="21"/>
     </row>
-    <row r="39" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A39" s="66"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
@@ -6564,7 +7225,7 @@
       <c r="I39" s="27"/>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A40" s="66"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
@@ -6574,7 +7235,7 @@
         <v>198</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H40" s="22" t="s">
         <v>18</v>
@@ -6584,7 +7245,7 @@
       </c>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A41" s="66"/>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
@@ -6598,7 +7259,7 @@
       <c r="I41" s="27"/>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A42" s="29" t="s">
         <v>211</v>
       </c>
@@ -6612,7 +7273,7 @@
         <v>196</v>
       </c>
       <c r="G42" s="46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H42" s="22" t="s">
         <v>18</v>
@@ -6622,7 +7283,7 @@
       </c>
       <c r="J42" s="21"/>
     </row>
-    <row r="43" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A43" s="66"/>
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
@@ -6636,7 +7297,7 @@
       <c r="I43" s="27"/>
       <c r="J43" s="21"/>
     </row>
-    <row r="44" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A44" s="66"/>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
@@ -6646,7 +7307,7 @@
         <v>197</v>
       </c>
       <c r="G44" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H44" s="22" t="s">
         <v>18</v>
@@ -6656,7 +7317,7 @@
       </c>
       <c r="J44" s="21"/>
     </row>
-    <row r="45" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A45" s="66"/>
       <c r="B45" s="23"/>
       <c r="C45" s="23"/>
@@ -6670,7 +7331,7 @@
       <c r="I45" s="27"/>
       <c r="J45" s="21"/>
     </row>
-    <row r="46" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A46" s="66"/>
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
@@ -6680,7 +7341,7 @@
         <v>198</v>
       </c>
       <c r="G46" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H46" s="22" t="s">
         <v>50</v>
@@ -6690,7 +7351,7 @@
       </c>
       <c r="J46" s="21"/>
     </row>
-    <row r="47" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A47" s="30"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
@@ -6704,7 +7365,7 @@
       <c r="I47" s="27"/>
       <c r="J47" s="21"/>
     </row>
-    <row r="48" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A48" s="66" t="s">
         <v>212</v>
       </c>
@@ -6718,7 +7379,7 @@
         <v>196</v>
       </c>
       <c r="G48" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H48" s="22" t="s">
         <v>17</v>
@@ -6728,7 +7389,7 @@
       </c>
       <c r="J48" s="21"/>
     </row>
-    <row r="49" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A49" s="66"/>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
@@ -6742,7 +7403,7 @@
       <c r="I49" s="27"/>
       <c r="J49" s="21"/>
     </row>
-    <row r="50" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A50" s="66"/>
       <c r="B50" s="67"/>
       <c r="C50" s="23"/>
@@ -6752,7 +7413,7 @@
         <v>197</v>
       </c>
       <c r="G50" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H50" s="22" t="s">
         <v>17</v>
@@ -6762,7 +7423,7 @@
       </c>
       <c r="J50" s="21"/>
     </row>
-    <row r="51" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A51" s="66"/>
       <c r="B51" s="67"/>
       <c r="C51" s="23"/>
@@ -6776,7 +7437,7 @@
       <c r="I51" s="27"/>
       <c r="J51" s="21"/>
     </row>
-    <row r="52" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A52" s="66"/>
       <c r="B52" s="67"/>
       <c r="C52" s="23"/>
@@ -6786,7 +7447,7 @@
         <v>198</v>
       </c>
       <c r="G52" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H52" s="22" t="s">
         <v>17</v>
@@ -6796,7 +7457,7 @@
       </c>
       <c r="J52" s="21"/>
     </row>
-    <row r="53" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A53" s="30"/>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
@@ -6810,7 +7471,7 @@
       <c r="I53" s="27"/>
       <c r="J53" s="21"/>
     </row>
-    <row r="54" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A54" s="58" t="s">
         <v>213</v>
       </c>
@@ -6824,7 +7485,7 @@
         <v>196</v>
       </c>
       <c r="G54" s="46" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H54" s="22" t="s">
         <v>187</v>
@@ -6834,7 +7495,7 @@
       </c>
       <c r="J54" s="21"/>
     </row>
-    <row r="55" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A55" s="23"/>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
@@ -6848,7 +7509,7 @@
       <c r="I55" s="27"/>
       <c r="J55" s="21"/>
     </row>
-    <row r="56" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A56" s="23"/>
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
@@ -6858,7 +7519,7 @@
         <v>197</v>
       </c>
       <c r="G56" s="46" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H56" s="22" t="s">
         <v>187</v>
@@ -6868,7 +7529,7 @@
       </c>
       <c r="J56" s="21"/>
     </row>
-    <row r="57" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A57" s="23"/>
       <c r="B57" s="23"/>
       <c r="C57" s="23"/>
@@ -6882,7 +7543,7 @@
       <c r="I57" s="27"/>
       <c r="J57" s="21"/>
     </row>
-    <row r="58" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A58" s="23"/>
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
@@ -6892,7 +7553,7 @@
         <v>198</v>
       </c>
       <c r="G58" s="46" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H58" s="22" t="s">
         <v>187</v>
@@ -6902,7 +7563,7 @@
       </c>
       <c r="J58" s="21"/>
     </row>
-    <row r="59" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A59" s="27"/>
       <c r="B59" s="27"/>
       <c r="C59" s="27"/>
@@ -6916,7 +7577,7 @@
       <c r="I59" s="27"/>
       <c r="J59" s="21"/>
     </row>
-    <row r="60" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A60" s="58" t="s">
         <v>214</v>
       </c>
@@ -6930,7 +7591,7 @@
         <v>196</v>
       </c>
       <c r="G60" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H60" s="22" t="s">
         <v>187</v>
@@ -6940,7 +7601,7 @@
       </c>
       <c r="J60" s="21"/>
     </row>
-    <row r="61" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A61" s="23"/>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
@@ -6954,7 +7615,7 @@
       <c r="I61" s="27"/>
       <c r="J61" s="21"/>
     </row>
-    <row r="62" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A62" s="23"/>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -6964,7 +7625,7 @@
         <v>197</v>
       </c>
       <c r="G62" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H62" s="22" t="s">
         <v>187</v>
@@ -6974,7 +7635,7 @@
       </c>
       <c r="J62" s="21"/>
     </row>
-    <row r="63" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A63" s="23"/>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
@@ -6988,7 +7649,7 @@
       <c r="I63" s="27"/>
       <c r="J63" s="21"/>
     </row>
-    <row r="64" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
@@ -6998,7 +7659,7 @@
         <v>198</v>
       </c>
       <c r="G64" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H64" s="22" t="s">
         <v>187</v>
@@ -7008,7 +7669,7 @@
       </c>
       <c r="J64" s="21"/>
     </row>
-    <row r="65" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A65" s="27"/>
       <c r="B65" s="27"/>
       <c r="C65" s="27"/>
@@ -7022,7 +7683,7 @@
       <c r="I65" s="27"/>
       <c r="J65" s="21"/>
     </row>
-    <row r="66" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A66" s="58" t="s">
         <v>215</v>
       </c>
@@ -7036,7 +7697,7 @@
         <v>196</v>
       </c>
       <c r="G66" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H66" s="22" t="s">
         <v>187</v>
@@ -7046,7 +7707,7 @@
       </c>
       <c r="J66" s="21"/>
     </row>
-    <row r="67" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
       <c r="C67" s="23"/>
@@ -7060,7 +7721,7 @@
       <c r="I67" s="27"/>
       <c r="J67" s="21"/>
     </row>
-    <row r="68" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A68" s="23"/>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
@@ -7070,7 +7731,7 @@
         <v>197</v>
       </c>
       <c r="G68" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H68" s="22" t="s">
         <v>187</v>
@@ -7080,7 +7741,7 @@
       </c>
       <c r="J68" s="21"/>
     </row>
-    <row r="69" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A69" s="23"/>
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
@@ -7094,7 +7755,7 @@
       <c r="I69" s="27"/>
       <c r="J69" s="21"/>
     </row>
-    <row r="70" spans="1:10" ht="78" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A70" s="23"/>
       <c r="B70" s="23"/>
       <c r="C70" s="23"/>
@@ -7104,7 +7765,7 @@
         <v>198</v>
       </c>
       <c r="G70" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H70" s="22" t="s">
         <v>187</v>
@@ -7114,7 +7775,7 @@
       </c>
       <c r="J70" s="21"/>
     </row>
-    <row r="71" spans="1:10" ht="65" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A71" s="27"/>
       <c r="B71" s="27"/>
       <c r="C71" s="27"/>
@@ -7143,52 +7804,52 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.90625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="41.7265625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="60.36328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="41.75" style="6" customWidth="1"/>
+    <col min="4" max="4" width="60.375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
         <v>12</v>
       </c>
@@ -7209,7 +7870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>54</v>
       </c>
@@ -7220,7 +7881,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>50</v>
@@ -7230,7 +7891,7 @@
       </c>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A11" s="30"/>
       <c r="B11" s="23"/>
       <c r="C11" s="27"/>
@@ -7241,7 +7902,7 @@
       <c r="F11" s="27"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>55</v>
       </c>
@@ -7250,7 +7911,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>18</v>
@@ -7260,7 +7921,7 @@
       </c>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A13" s="30"/>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
@@ -7271,7 +7932,7 @@
       <c r="F13" s="27"/>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>56</v>
       </c>
@@ -7282,7 +7943,7 @@
         <v>51</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>50</v>
@@ -7292,7 +7953,7 @@
       </c>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A15" s="30"/>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
@@ -7318,32 +7979,32 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="35.90625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="37.08984375" customWidth="1"/>
-    <col min="4" max="4" width="59.90625" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="35.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.125" customWidth="1"/>
+    <col min="4" max="4" width="59.875" customWidth="1"/>
+    <col min="5" max="5" width="19.125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="20.25" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="37"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>62</v>
@@ -7351,7 +8012,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>63</v>
@@ -7359,14 +8020,14 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>118</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
         <v>188</v>
@@ -7374,7 +8035,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>120</v>
@@ -7382,7 +8043,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>121</v>
@@ -7390,12 +8051,12 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -7416,7 +8077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>59</v>
       </c>
@@ -7427,7 +8088,7 @@
         <v>113</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>50</v>
@@ -7437,7 +8098,7 @@
       </c>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="30"/>
       <c r="B12" s="23"/>
       <c r="C12" s="27"/>
@@ -7448,7 +8109,7 @@
       <c r="F12" s="27"/>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>112</v>
       </c>
@@ -7459,7 +8120,7 @@
         <v>105</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>18</v>
@@ -7469,7 +8130,7 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A14" s="27"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -7480,7 +8141,7 @@
       <c r="F14" s="27"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
         <v>116</v>
       </c>
@@ -7491,7 +8152,7 @@
         <v>114</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>50</v>
@@ -7501,7 +8162,7 @@
       </c>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A16" s="30"/>
       <c r="B16" s="23"/>
       <c r="C16" s="27"/>
@@ -7512,7 +8173,7 @@
       <c r="F16" s="27"/>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A17" s="43" t="s">
         <v>117</v>
       </c>
@@ -7523,7 +8184,7 @@
         <v>136</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>18</v>
@@ -7533,7 +8194,7 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
@@ -7558,17 +8219,17 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="39.453125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="41.6328125" customWidth="1"/>
-    <col min="4" max="4" width="63.26953125" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" customWidth="1"/>
-    <col min="6" max="6" width="22.90625" customWidth="1"/>
-    <col min="7" max="7" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41.625" customWidth="1"/>
+    <col min="4" max="4" width="63.25" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="22.875" customWidth="1"/>
+    <col min="7" max="7" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -7579,7 +8240,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -7590,7 +8251,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
@@ -7601,7 +8262,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="19" t="s">
         <v>64</v>
@@ -7612,7 +8273,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="19" t="s">
         <v>63</v>
@@ -7623,7 +8284,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="19" t="s">
         <v>65</v>
@@ -7634,7 +8295,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>118</v>
       </c>
@@ -7644,7 +8305,7 @@
       <c r="E7" s="10"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="19" t="s">
         <v>62</v>
@@ -7654,7 +8315,7 @@
       <c r="E8" s="10"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="19" t="s">
         <v>122</v>
@@ -7664,7 +8325,7 @@
       <c r="E9" s="10"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
         <v>119</v>
@@ -7674,7 +8335,7 @@
       <c r="E10" s="10"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>189</v>
@@ -7684,7 +8345,7 @@
       <c r="E11" s="10"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
         <v>120</v>
@@ -7694,7 +8355,7 @@
       <c r="E12" s="10"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
         <v>121</v>
@@ -7704,7 +8365,7 @@
       <c r="E13" s="10"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -7713,7 +8374,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
         <v>12</v>
       </c>
@@ -7734,7 +8395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A16" s="68" t="s">
         <v>73</v>
       </c>
@@ -7745,7 +8406,7 @@
         <v>106</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E16" s="71" t="s">
         <v>50</v>
@@ -7755,7 +8416,7 @@
       </c>
       <c r="G16" s="70"/>
     </row>
-    <row r="17" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A17" s="72"/>
       <c r="B17" s="73"/>
       <c r="C17" s="73"/>
@@ -7766,7 +8427,7 @@
       <c r="F17" s="74"/>
       <c r="G17" s="70"/>
     </row>
-    <row r="18" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>74</v>
       </c>
@@ -7777,7 +8438,7 @@
         <v>107</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>18</v>
@@ -7787,7 +8448,7 @@
       </c>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -7798,7 +8459,7 @@
       <c r="F19" s="14"/>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="56.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
@@ -7809,7 +8470,7 @@
         <v>108</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>18</v>
@@ -7819,7 +8480,7 @@
       </c>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
       <c r="B21" s="18"/>
       <c r="C21" s="8"/>
@@ -7830,7 +8491,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A22" s="44" t="s">
         <v>129</v>
       </c>
@@ -7841,7 +8502,7 @@
         <v>125</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E22" s="47" t="s">
         <v>50</v>
@@ -7851,7 +8512,7 @@
       </c>
       <c r="G22" s="46"/>
     </row>
-    <row r="23" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A23" s="48"/>
       <c r="B23" s="49"/>
       <c r="C23" s="49"/>
@@ -7862,7 +8523,7 @@
       <c r="F23" s="52"/>
       <c r="G23" s="46"/>
     </row>
-    <row r="24" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A24" s="44" t="s">
         <v>130</v>
       </c>
@@ -7873,7 +8534,7 @@
         <v>124</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>18</v>
@@ -7883,7 +8544,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A25" s="48"/>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
@@ -7894,7 +8555,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A26" s="44" t="s">
         <v>131</v>
       </c>
@@ -7905,7 +8566,7 @@
         <v>128</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E26" s="47" t="s">
         <v>50</v>
@@ -7915,7 +8576,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A27" s="48"/>
       <c r="B27" s="18"/>
       <c r="C27" s="8"/>
@@ -7926,7 +8587,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A28" s="44" t="s">
         <v>132</v>
       </c>
@@ -7937,7 +8598,7 @@
         <v>127</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>18</v>
@@ -7947,7 +8608,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A29" s="48"/>
       <c r="B29" s="18"/>
       <c r="C29" s="8"/>
@@ -7972,18 +8633,18 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" customWidth="1"/>
-    <col min="3" max="3" width="44.08984375" customWidth="1"/>
-    <col min="4" max="4" width="63.90625" customWidth="1"/>
-    <col min="5" max="5" width="22.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="3" max="3" width="44.125" customWidth="1"/>
+    <col min="4" max="4" width="63.875" customWidth="1"/>
+    <col min="5" max="5" width="22.125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -7992,7 +8653,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -8001,7 +8662,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="19" t="s">
         <v>62</v>
@@ -8010,7 +8671,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="19" t="s">
         <v>122</v>
@@ -8019,7 +8680,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="19" t="s">
         <v>164</v>
@@ -8028,14 +8689,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
@@ -8056,7 +8717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A8" s="60" t="s">
         <v>76</v>
       </c>
@@ -8067,7 +8728,7 @@
         <v>167</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E8" s="61" t="s">
         <v>161</v>
@@ -8077,7 +8738,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="64"/>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
@@ -8090,7 +8751,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A10" s="60" t="s">
         <v>163</v>
       </c>
@@ -8101,7 +8762,7 @@
         <v>184</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E10" s="61" t="s">
         <v>162</v>
@@ -8111,7 +8772,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A11" s="64"/>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>

</xml_diff>

<commit_message>
Updated test spec document.
</commit_message>
<xml_diff>
--- a/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
+++ b/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
@@ -2684,44 +2684,6 @@
 % ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
   </si>
   <si>
-    <t>* 不正な中間認証局から発行したサーバ証明書: ./test_dir/A/server2/server.crt</t>
-    <rPh sb="2" eb="4">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>チュウカン</t>
-    </rPh>
-    <rPh sb="7" eb="10">
-      <t>ニンショウキョク</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ハッコウ</t>
-    </rPh>
-    <rPh sb="19" eb="22">
-      <t>ショウメイショ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">* 不正な中間認証局から発行したクライアント証明書: ./test_dir/B/client2/client.crt </t>
-    <rPh sb="2" eb="4">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>チュウカン</t>
-    </rPh>
-    <rPh sb="7" eb="10">
-      <t>ニンショウキョク</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ハッコウ</t>
-    </rPh>
-    <rPh sb="22" eb="25">
-      <t>ショウメイショ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">不正な中間認証局から発行したクライアント証明書を指定
 </t>
     <rPh sb="0" eb="2">
@@ -2748,11 +2710,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>テストサーバー起動
-% ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server2/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server2/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all2 --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>不正な中間認証局から発行した証明書</t>
     <rPh sb="14" eb="17">
       <t>ショウメイショ</t>
@@ -2812,45 +2769,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>テストクライアント起動
-% ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client2/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client2/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all2 --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>不正な中間認証局から発行したクライアント証明書を指定する。
-サーバ側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
-クライアント側の --tls_certificate_file、--tls_key_fileには B/client2/client.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all2 を指定する。</t>
-    <rPh sb="143" eb="144">
-      <t>ガワ</t>
-    </rPh>
-    <rPh sb="261" eb="263">
-      <t>シテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>テストサーバー起動
 % ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
   </si>
   <si>
     <t>テストサーバー起動
 % ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>不正な中間認証局から発行したクライアント証明書を指定する。
-クライアン側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。
-サーバ側の --tls_certificate_file、--tls_key_fileには B/server2/server.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all2 を指定する。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストサーバー起動
-% ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server2/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server2/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all2 --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストクライアント起動
-% ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client2/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client2/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all2 --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/A/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2898,12 +2822,6 @@
   <si>
     <t>テストクライアント起動
 % ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/A/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>不正な中間認証局から発行したサーバ・クライアント証明書を指定する。
-サーバ側の --tls_certificate_file、--tls_key_fileには B/server2/server.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all2、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
-クライアント側の --tls_certificate_file、--tls_key_fileには B/client2/client.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all2、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3027,6 +2945,82 @@
     <t>テストクライアント起動
 % ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>* 不正な中間認証局から発行したサーバ証明書: ./test_dir/A/server_under_inter_ca_4/server.crt</t>
+    <rPh sb="2" eb="4">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チュウカン</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ニンショウキョク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ハッコウ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ショウメイショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 不正な中間認証局から発行したクライアント証明書: ./test_dir/B/client_under_inter_ca_4/client.crt </t>
+    <rPh sb="2" eb="4">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チュウカン</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ニンショウキョク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ハッコウ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>ショウメイショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不正な中間認証局から発行したクライアント証明書を指定する。
+サーバ側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
+クライアント側の --tls_certificate_file、--tls_key_fileには B/client_under_inter_ca_4/client.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all_under_inter_ca_4 を指定する。</t>
+    <rPh sb="141" eb="142">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="291" eb="293">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all_under_inter_ca_4 --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
+  </si>
+  <si>
+    <t>不正な中間認証局から発行したクライアント証明書を指定する。
+クライアン側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。
+サーバ側の --tls_certificate_file、--tls_key_fileには B/server_under_inter_ca_4/server.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all_under_inter_ca_4 を指定する。</t>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server_under_inter_ca_4/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server_under_inter_ca_4/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all_under_inter_ca_4 --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
+  </si>
+  <si>
+    <t>不正な中間認証局から発行したサーバ・クライアント証明書を指定する。
+サーバ側の --tls_certificate_file、--tls_key_fileには B/server_under_inter_ca_4/server.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all_under_inter_ca_4、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
+クライアント側の --tls_certificate_file、--tls_key_fileには B/client_under_inter_ca_4/client.{crt,key}、 --tls_ca_certificate_path には A_B/cacerts_all_under_inter_ca_4、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
+  </si>
+  <si>
+    <t>テストサーバー起動
+% ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server_under_inter_ca_4/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server_under_inter_ca_4/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all_under_inter_ca_4 --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
+  </si>
+  <si>
+    <t>テストクライアント起動
+% ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all_under_inter_ca_4 --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/A/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
   </si>
 </sst>
 </file>
@@ -7260,12 +7254,12 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
@@ -9482,8 +9476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9561,7 +9555,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="89"/>
       <c r="B7" s="10" t="s">
-        <v>384</v>
+        <v>417</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -9571,7 +9565,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="89"/>
       <c r="B8" s="10" t="s">
-        <v>385</v>
+        <v>418</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -9619,10 +9613,10 @@
         <v>370</v>
       </c>
       <c r="D11" s="86" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F11" s="63" t="s">
         <v>155</v>
@@ -9632,7 +9626,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A12" s="92"/>
       <c r="B12" s="87"/>
       <c r="C12" s="67"/>
@@ -9644,7 +9638,7 @@
       <c r="G12" s="67"/>
       <c r="H12" s="64"/>
     </row>
-    <row r="13" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A13" s="93" t="s">
         <v>355</v>
       </c>
@@ -9653,10 +9647,10 @@
         <v>371</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>155</v>
@@ -9664,7 +9658,7 @@
       <c r="G13" s="87"/>
       <c r="H13" s="64"/>
     </row>
-    <row r="14" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A14" s="93"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -9676,7 +9670,7 @@
       <c r="G14" s="87"/>
       <c r="H14" s="64"/>
     </row>
-    <row r="15" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A15" s="91" t="s">
         <v>356</v>
       </c>
@@ -9687,10 +9681,10 @@
         <v>370</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="E15" s="64" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="F15" s="63" t="s">
         <v>156</v>
@@ -9698,7 +9692,7 @@
       <c r="G15" s="63"/>
       <c r="H15" s="64"/>
     </row>
-    <row r="16" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A16" s="92"/>
       <c r="B16" s="87"/>
       <c r="C16" s="67"/>
@@ -9710,7 +9704,7 @@
       <c r="G16" s="67"/>
       <c r="H16" s="64"/>
     </row>
-    <row r="17" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A17" s="91" t="s">
         <v>357</v>
       </c>
@@ -9719,10 +9713,10 @@
         <v>371</v>
       </c>
       <c r="D17" s="86" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="F17" s="63" t="s">
         <v>156</v>
@@ -9730,7 +9724,7 @@
       <c r="G17" s="63"/>
       <c r="H17" s="64"/>
     </row>
-    <row r="18" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A18" s="92"/>
       <c r="B18" s="87"/>
       <c r="C18" s="87"/>
@@ -9753,7 +9747,7 @@
         <v>370</v>
       </c>
       <c r="D19" s="86" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E19" s="64" t="s">
         <v>383</v>
@@ -9764,13 +9758,13 @@
       <c r="G19" s="63"/>
       <c r="H19" s="64"/>
     </row>
-    <row r="20" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A20" s="92"/>
       <c r="B20" s="87"/>
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
       <c r="E20" s="64" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="67"/>
@@ -9785,7 +9779,7 @@
         <v>371</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="E21" s="64" t="s">
         <v>383</v>
@@ -9796,13 +9790,13 @@
       <c r="G21" s="87"/>
       <c r="H21" s="64"/>
     </row>
-    <row r="22" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A22" s="93"/>
       <c r="B22" s="87"/>
       <c r="C22" s="87"/>
       <c r="D22" s="87"/>
       <c r="E22" s="64" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="F22" s="87"/>
       <c r="G22" s="87"/>
@@ -9819,7 +9813,7 @@
         <v>370</v>
       </c>
       <c r="D23" s="86" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>383</v>
@@ -9830,13 +9824,13 @@
       <c r="G23" s="63"/>
       <c r="H23" s="64"/>
     </row>
-    <row r="24" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A24" s="92"/>
       <c r="B24" s="87"/>
       <c r="C24" s="67"/>
       <c r="D24" s="67"/>
       <c r="E24" s="64" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="67"/>
@@ -9851,7 +9845,7 @@
         <v>371</v>
       </c>
       <c r="D25" s="86" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="E25" s="64" t="s">
         <v>383</v>
@@ -9862,13 +9856,13 @@
       <c r="G25" s="63"/>
       <c r="H25" s="64"/>
     </row>
-    <row r="26" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A26" s="92"/>
       <c r="B26" s="87"/>
       <c r="C26" s="87"/>
       <c r="D26" s="67"/>
       <c r="E26" s="64" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F26" s="67"/>
       <c r="G26" s="67"/>
@@ -9885,10 +9879,10 @@
         <v>370</v>
       </c>
       <c r="D27" s="86" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F27" s="63" t="s">
         <v>155</v>
@@ -9896,13 +9890,13 @@
       <c r="G27" s="63"/>
       <c r="H27" s="64"/>
     </row>
-    <row r="28" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A28" s="92"/>
       <c r="B28" s="87"/>
       <c r="C28" s="67"/>
       <c r="D28" s="67"/>
       <c r="E28" s="64" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="F28" s="67"/>
       <c r="G28" s="67"/>
@@ -9917,10 +9911,10 @@
         <v>371</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="F29" s="63" t="s">
         <v>155</v>
@@ -9928,13 +9922,13 @@
       <c r="G29" s="87"/>
       <c r="H29" s="64"/>
     </row>
-    <row r="30" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A30" s="93"/>
       <c r="B30" s="87"/>
       <c r="C30" s="87"/>
       <c r="D30" s="87"/>
       <c r="E30" s="64" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="F30" s="87"/>
       <c r="G30" s="87"/>
@@ -9951,10 +9945,10 @@
         <v>370</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="F31" s="63" t="s">
         <v>156</v>
@@ -9968,7 +9962,7 @@
       <c r="C32" s="67"/>
       <c r="D32" s="67"/>
       <c r="E32" s="64" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="F32" s="67"/>
       <c r="G32" s="67"/>
@@ -9983,10 +9977,10 @@
         <v>371</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="E33" s="64" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="F33" s="63" t="s">
         <v>156</v>
@@ -10000,7 +9994,7 @@
       <c r="C34" s="67"/>
       <c r="D34" s="67"/>
       <c r="E34" s="64" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F34" s="67"/>
       <c r="G34" s="67"/>
@@ -10008,19 +10002,19 @@
     </row>
     <row r="35" spans="1:8" ht="135" x14ac:dyDescent="0.15">
       <c r="A35" s="91" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B35" s="87" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C35" s="86" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>392</v>
+        <v>419</v>
       </c>
       <c r="E35" s="64" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F35" s="63" t="s">
         <v>156</v>
@@ -10034,7 +10028,7 @@
       <c r="C36" s="87"/>
       <c r="D36" s="67"/>
       <c r="E36" s="64" t="s">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="F36" s="67"/>
       <c r="G36" s="67"/>
@@ -10042,17 +10036,17 @@
     </row>
     <row r="37" spans="1:8" ht="135" x14ac:dyDescent="0.15">
       <c r="A37" s="91" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B37" s="87"/>
       <c r="C37" s="86" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D37" s="86" t="s">
-        <v>395</v>
+        <v>421</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>387</v>
+        <v>422</v>
       </c>
       <c r="F37" s="63" t="s">
         <v>156</v>
@@ -10066,7 +10060,7 @@
       <c r="C38" s="87"/>
       <c r="D38" s="67"/>
       <c r="E38" s="64" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="F38" s="67"/>
       <c r="G38" s="67"/>
@@ -10074,17 +10068,17 @@
     </row>
     <row r="39" spans="1:8" ht="162" x14ac:dyDescent="0.15">
       <c r="A39" s="91" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B39" s="87"/>
       <c r="C39" s="86" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D39" s="86" t="s">
-        <v>402</v>
+        <v>423</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
       <c r="F39" s="63" t="s">
         <v>156</v>
@@ -10098,7 +10092,7 @@
       <c r="C40" s="67"/>
       <c r="D40" s="67"/>
       <c r="E40" s="64" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
       <c r="F40" s="67"/>
       <c r="G40" s="67"/>

</xml_diff>

<commit_message>
Deleted test 6-2, 6-6, and 6-10
</commit_message>
<xml_diff>
--- a/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
+++ b/regress/manual/lib/libgfarm/gfarm/tls-test/test-specs-JP/gfarm_tls_test.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="418">
   <si>
     <t>証明書</t>
     <rPh sb="0" eb="3">
@@ -2467,18 +2467,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>6-3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>6-4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>6-5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>6-7</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2500,10 +2492,6 @@
   </si>
   <si>
     <t>6-10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6-12</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2825,28 +2813,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>6-13</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6-14</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6-15</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>tls_ca_peer_verify_chain_path にクライアント側の正しいルート証明書を指定する。
 サーバ側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。</t>
-  </si>
-  <si>
-    <t>tls_ca_peer_verify_chain_path にクライアント側の正しいルート証明書を指定する。
-サーバ側の --tls_ca_certificate_path にはA/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。</t>
-  </si>
-  <si>
-    <t>テストサーバー起動
-% ./tls-test -s --tls_certificate_file ./test_dir/verify_chain_path/A/server/server.crt --tls_key_file ./test_dir/verify_chain_path/A/server/server.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/B/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
   </si>
   <si>
     <t>tls_ca_peer_verify_chain_path にクライアント側の不正なルート証明書を指定する。
@@ -2877,14 +2845,6 @@
 クライアン側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
   </si>
   <si>
-    <t>tls_ca_peer_verify_chain_path にサーバ側の正しいルート証明書を指定する。
-クライアン側の --tls_ca_certificate_path にはB/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
-  </si>
-  <si>
-    <t>テストクライアント起動
-% ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/B/cacerts_all --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/A/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
-  </si>
-  <si>
     <t>tls_ca_peer_verify_chain_path にサーバ側の不正なルート証明書を指定する。
 クライアン側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。</t>
     <rPh sb="34" eb="36">
@@ -2912,11 +2872,6 @@
     <t>tls_ca_peer_verify_chain_path にそれぞれサーバ・クライアントの正しいルート証明書を指定する。
 サーバ側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
 クライアン側の --tls_ca_certificate_path にはA_B/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
-  </si>
-  <si>
-    <t>tls_ca_peer_verify_chain_path にそれぞれサーバ・クライアントの正しいルート証明書を指定する。
-サーバ側の --tls_ca_certificate_path にはA/cacerts_all、--tls_ca_peer_verify_chain_path には B/cacerts_all を指定する。
-クライアン側の --tls_ca_certificate_path にはB/cacerts_all、--tls_ca_peer_verify_chain_path には A/cacerts_all を指定する。</t>
   </si>
   <si>
     <t>tls_ca_peer_verify_chain_path にそれぞれサーバ・クライアントの不正なルート証明書を指定する。
@@ -3021,6 +2976,18 @@
   <si>
     <t>テストクライアント起動
 % ./tls-test --tls_certificate_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.crt --tls_key_file ./test_dir/verify_chain_path/B/client_under_inter_ca_4/client.key --tls_ca_certificate_path ./test_dir/verify_chain_path/A_B/cacerts_all_under_inter_ca_4 --tls_ca_peer_verify_chain_path ./test_dir/verify_chain_path/A/cacerts_all --once --mutual_authentication --allow_no_crl --build_chain --debug_level 1 --verify_only</t>
+  </si>
+  <si>
+    <t>6-3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6-5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6-12</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -3259,7 +3226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3513,9 +3480,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6299,7 +6263,7 @@
     <row r="7" spans="1:8" s="55" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6406,13 +6370,13 @@
         <v>163</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E14" s="57" t="s">
         <v>91</v>
@@ -7254,12 +7218,12 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
@@ -7388,7 +7352,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -9474,15 +9438,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="94" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="93" customWidth="1"/>
     <col min="2" max="2" width="41.125" customWidth="1"/>
     <col min="3" max="3" width="30.375" customWidth="1"/>
     <col min="4" max="4" width="44.125" customWidth="1"/>
@@ -9535,7 +9499,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="89"/>
       <c r="B5" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -9545,7 +9509,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="89"/>
       <c r="B6" s="10" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -9555,7 +9519,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="89"/>
       <c r="B7" s="10" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -9565,7 +9529,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="89"/>
       <c r="B8" s="10" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -9607,23 +9571,23 @@
         <v>354</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C11" s="86" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D11" s="86" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F11" s="63" t="s">
         <v>155</v>
       </c>
       <c r="G11" s="63"/>
-      <c r="H11" s="95" t="s">
-        <v>368</v>
+      <c r="H11" s="94" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="81" x14ac:dyDescent="0.15">
@@ -9632,59 +9596,59 @@
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
       <c r="E12" s="64" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F12" s="67"/>
       <c r="G12" s="67"/>
       <c r="H12" s="64"/>
     </row>
     <row r="13" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="91" t="s">
         <v>355</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="88" t="s">
-        <v>371</v>
+      <c r="B13" s="63" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>367</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="G13" s="87"/>
+        <v>156</v>
+      </c>
+      <c r="G13" s="63"/>
       <c r="H13" s="64"/>
     </row>
     <row r="14" spans="1:8" ht="81" x14ac:dyDescent="0.15">
-      <c r="A14" s="93"/>
+      <c r="A14" s="92"/>
       <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="64" t="s">
-        <v>382</v>
-      </c>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+        <v>379</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="64"/>
     </row>
     <row r="15" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A15" s="91" t="s">
-        <v>356</v>
-      </c>
-      <c r="B15" s="63" t="s">
-        <v>372</v>
-      </c>
-      <c r="C15" s="86" t="s">
-        <v>370</v>
+        <v>415</v>
+      </c>
+      <c r="B15" s="87"/>
+      <c r="C15" s="88" t="s">
+        <v>368</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="E15" s="64" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F15" s="63" t="s">
         <v>156</v>
@@ -9695,65 +9659,67 @@
     <row r="16" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A16" s="92"/>
       <c r="B16" s="87"/>
-      <c r="C16" s="67"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="67"/>
       <c r="E16" s="64" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="67"/>
       <c r="H16" s="64"/>
     </row>
-    <row r="17" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="81" x14ac:dyDescent="0.15">
       <c r="A17" s="91" t="s">
-        <v>357</v>
-      </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="88" t="s">
-        <v>371</v>
+        <v>356</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>370</v>
+      </c>
+      <c r="C17" s="86" t="s">
+        <v>367</v>
       </c>
       <c r="D17" s="86" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E17" s="64" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="F17" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G17" s="63"/>
       <c r="H17" s="64"/>
     </row>
-    <row r="18" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A18" s="92"/>
       <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="67"/>
       <c r="E18" s="64" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="67"/>
       <c r="H18" s="64"/>
     </row>
-    <row r="19" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A19" s="91" t="s">
-        <v>358</v>
+        <v>416</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C19" s="86" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D19" s="86" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F19" s="63" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G19" s="63"/>
       <c r="H19" s="64"/>
@@ -9764,62 +9730,62 @@
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
       <c r="E20" s="64" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="67"/>
       <c r="H20" s="64"/>
     </row>
     <row r="21" spans="1:8" ht="81" x14ac:dyDescent="0.15">
-      <c r="A21" s="93" t="s">
-        <v>362</v>
+      <c r="A21" s="91" t="s">
+        <v>360</v>
       </c>
       <c r="B21" s="87"/>
       <c r="C21" s="88" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F21" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="G21" s="87"/>
+        <v>156</v>
+      </c>
+      <c r="G21" s="63"/>
       <c r="H21" s="64"/>
     </row>
     <row r="22" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="93"/>
+      <c r="A22" s="92"/>
       <c r="B22" s="87"/>
       <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="64" t="s">
-        <v>406</v>
-      </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+        <v>400</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="64"/>
     </row>
-    <row r="23" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A23" s="91" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C23" s="86" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D23" s="86" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F23" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G23" s="63"/>
       <c r="H23" s="64"/>
@@ -9830,25 +9796,27 @@
       <c r="C24" s="67"/>
       <c r="D24" s="67"/>
       <c r="E24" s="64" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="F24" s="67"/>
       <c r="G24" s="67"/>
       <c r="H24" s="64"/>
     </row>
-    <row r="25" spans="1:8" ht="81" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A25" s="91" t="s">
-        <v>360</v>
-      </c>
-      <c r="B25" s="87"/>
-      <c r="C25" s="88" t="s">
-        <v>371</v>
+        <v>358</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>373</v>
+      </c>
+      <c r="C25" s="86" t="s">
+        <v>367</v>
       </c>
       <c r="D25" s="86" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="F25" s="63" t="s">
         <v>156</v>
@@ -9859,10 +9827,10 @@
     <row r="26" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A26" s="92"/>
       <c r="B26" s="87"/>
-      <c r="C26" s="87"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="67"/>
       <c r="E26" s="64" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F26" s="67"/>
       <c r="G26" s="67"/>
@@ -9870,85 +9838,83 @@
     </row>
     <row r="27" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A27" s="91" t="s">
-        <v>363</v>
-      </c>
-      <c r="B27" s="63" t="s">
-        <v>375</v>
-      </c>
-      <c r="C27" s="86" t="s">
-        <v>370</v>
+        <v>361</v>
+      </c>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88" t="s">
+        <v>368</v>
       </c>
       <c r="D27" s="86" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="F27" s="63" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G27" s="63"/>
       <c r="H27" s="64"/>
     </row>
     <row r="28" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A28" s="92"/>
-      <c r="B28" s="87"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="67"/>
       <c r="D28" s="67"/>
       <c r="E28" s="64" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="F28" s="67"/>
       <c r="G28" s="67"/>
       <c r="H28" s="64"/>
     </row>
-    <row r="29" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="93" t="s">
-        <v>364</v>
-      </c>
-      <c r="B29" s="87"/>
-      <c r="C29" s="88" t="s">
-        <v>371</v>
+    <row r="29" spans="1:8" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A29" s="91" t="s">
+        <v>362</v>
+      </c>
+      <c r="B29" s="87" t="s">
+        <v>382</v>
+      </c>
+      <c r="C29" s="86" t="s">
+        <v>381</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E29" s="64" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F29" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="G29" s="87"/>
+        <v>156</v>
+      </c>
+      <c r="G29" s="63"/>
       <c r="H29" s="64"/>
     </row>
-    <row r="30" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A30" s="93"/>
+    <row r="30" spans="1:8" ht="108" x14ac:dyDescent="0.15">
+      <c r="A30" s="92"/>
       <c r="B30" s="87"/>
       <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
+      <c r="D30" s="67"/>
       <c r="E30" s="64" t="s">
-        <v>406</v>
-      </c>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
+        <v>409</v>
+      </c>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
       <c r="H30" s="64"/>
     </row>
-    <row r="31" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A31" s="91" t="s">
-        <v>361</v>
-      </c>
-      <c r="B31" s="63" t="s">
-        <v>376</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="B31" s="87"/>
       <c r="C31" s="86" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E31" s="64" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F31" s="63" t="s">
         <v>156</v>
@@ -9959,28 +9925,28 @@
     <row r="32" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A32" s="92"/>
       <c r="B32" s="87"/>
-      <c r="C32" s="67"/>
+      <c r="C32" s="87"/>
       <c r="D32" s="67"/>
       <c r="E32" s="64" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="F32" s="67"/>
       <c r="G32" s="67"/>
       <c r="H32" s="64"/>
     </row>
-    <row r="33" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="216" x14ac:dyDescent="0.15">
       <c r="A33" s="91" t="s">
-        <v>365</v>
+        <v>417</v>
       </c>
       <c r="B33" s="87"/>
-      <c r="C33" s="88" t="s">
-        <v>371</v>
+      <c r="C33" s="86" t="s">
+        <v>383</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E33" s="64" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="F33" s="63" t="s">
         <v>156</v>
@@ -9988,115 +9954,17 @@
       <c r="G33" s="63"/>
       <c r="H33" s="64"/>
     </row>
-    <row r="34" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A34" s="92"/>
       <c r="B34" s="67"/>
       <c r="C34" s="67"/>
       <c r="D34" s="67"/>
       <c r="E34" s="64" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="F34" s="67"/>
       <c r="G34" s="67"/>
       <c r="H34" s="64"/>
-    </row>
-    <row r="35" spans="1:8" ht="135" x14ac:dyDescent="0.15">
-      <c r="A35" s="91" t="s">
-        <v>394</v>
-      </c>
-      <c r="B35" s="87" t="s">
-        <v>385</v>
-      </c>
-      <c r="C35" s="86" t="s">
-        <v>384</v>
-      </c>
-      <c r="D35" s="86" t="s">
-        <v>419</v>
-      </c>
-      <c r="E35" s="64" t="s">
-        <v>389</v>
-      </c>
-      <c r="F35" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-    </row>
-    <row r="36" spans="1:8" ht="81" x14ac:dyDescent="0.15">
-      <c r="A36" s="92"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="64" t="s">
-        <v>420</v>
-      </c>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="64"/>
-    </row>
-    <row r="37" spans="1:8" ht="135" x14ac:dyDescent="0.15">
-      <c r="A37" s="91" t="s">
-        <v>395</v>
-      </c>
-      <c r="B37" s="87"/>
-      <c r="C37" s="86" t="s">
-        <v>387</v>
-      </c>
-      <c r="D37" s="86" t="s">
-        <v>421</v>
-      </c>
-      <c r="E37" s="64" t="s">
-        <v>422</v>
-      </c>
-      <c r="F37" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" s="63"/>
-      <c r="H37" s="64"/>
-    </row>
-    <row r="38" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A38" s="92"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="64" t="s">
-        <v>393</v>
-      </c>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="64"/>
-    </row>
-    <row r="39" spans="1:8" ht="162" x14ac:dyDescent="0.15">
-      <c r="A39" s="91" t="s">
-        <v>396</v>
-      </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="86" t="s">
-        <v>386</v>
-      </c>
-      <c r="D39" s="86" t="s">
-        <v>423</v>
-      </c>
-      <c r="E39" s="64" t="s">
-        <v>424</v>
-      </c>
-      <c r="F39" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="G39" s="63"/>
-      <c r="H39" s="64"/>
-    </row>
-    <row r="40" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="92"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="64" t="s">
-        <v>425</v>
-      </c>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>